<commit_message>
ZIP. Remove parentheses method and tests.
</commit_message>
<xml_diff>
--- a/excelFiles/MyIT_Status.xlsx
+++ b/excelFiles/MyIT_Status.xlsx
@@ -81,7 +81,7 @@
     <t>INC44624294</t>
   </si>
   <si>
-    <t>Kostovski, Simon (GBS CEE FPS CZ AS FSD 3)</t>
+    <t>Kostovski, Simon</t>
   </si>
   <si>
     <t>please update the status for DP 31723 document to posted, it has been already approved</t>
@@ -113,7 +113,7 @@
     <t>INC44581236</t>
   </si>
   <si>
-    <t>Øhrgaard, Maria Karmark (SMO NEE RC-DK PC)</t>
+    <t>Øhrgaard, Maria Karmark</t>
   </si>
   <si>
     <t>Supplier credit note goes to wrong PO</t>
@@ -136,7 +136,7 @@
     <t>INC44557114</t>
   </si>
   <si>
-    <t>Tsakova, Konstantina (GBS CEE FPS CZ PR FS 2)</t>
+    <t>Tsakova, Konstantina</t>
   </si>
   <si>
     <t>Don't receive attachments in email</t>
@@ -163,7 +163,7 @@
     <t>INC44475191</t>
   </si>
   <si>
-    <t>Piedade, Pedro (CF R WEA PP SPE 1)</t>
+    <t>Piedade, Pedro</t>
   </si>
   <si>
     <t>Tax code is inconsistent in VIM when compared with PO</t>
@@ -179,7 +179,7 @@
     <t>INC44247133</t>
   </si>
   <si>
-    <t>Polanská, Pavlína (GBS CEE FPS CZ PR DIR 2)</t>
+    <t>Polanská, Pavlína</t>
   </si>
   <si>
     <t>Inbox don't work properly</t>
@@ -195,7 +195,7 @@
     <t>INC44233598</t>
   </si>
   <si>
-    <t>Prasad K, Nagendra (GBS ASP FPS RPM PD2)</t>
+    <t>Prasad K, Nagendra</t>
   </si>
   <si>
     <t>Vendor bills on ISD registration not getting captured.</t>
@@ -216,7 +216,7 @@
     <t>INC43708822</t>
   </si>
   <si>
-    <t>Wessner, Anna (DI MC MF GVC SCE SE)</t>
+    <t>Wessner, Anna</t>
   </si>
   <si>
     <t>No transparency in Order Confirmation Workflow</t>

</xml_diff>

<commit_message>
Tickets are put in order of creation. Tickets that are not VIM are now Ignored. Denmark is automatically changed to the correct ARE Mobility...
</commit_message>
<xml_diff>
--- a/excelFiles/MyIT_Status.xlsx
+++ b/excelFiles/MyIT_Status.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t>Control Date</t>
   </si>
@@ -78,25 +78,139 @@
     <t>Buzias</t>
   </si>
   <si>
-    <t>INC44624294</t>
+    <t>INC43607409</t>
+  </si>
+  <si>
+    <t>Tomisová, Ivana</t>
+  </si>
+  <si>
+    <t>3014 – issue with workflow approval process – Error in stating approval workflow</t>
+  </si>
+  <si>
+    <t>3014 - SIMEA BUZ</t>
+  </si>
+  <si>
+    <t>3 - Medium</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Dear colleagues,
+Please check the attachements with documents that we have issue with starting approval process.
+Thank you and kind regards
+Ivana</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>INC44483028</t>
+  </si>
+  <si>
+    <t>Høy, Niels-Erik</t>
+  </si>
+  <si>
+    <t>Not possible to approve invoices on added items to migrated FO</t>
+  </si>
+  <si>
+    <t>3012 - Siemens Mobility A/S</t>
+  </si>
+  <si>
+    <t>Please provide details about the nature of your issue.
+Description of the Issue
+Is process “Adding new time to existing FO” no longer allowed or is it only for migrated FO the process is no longer allowed?
+When we add a new item to a migrated FO, invoices can be booked but not approved because the limit is exceeded.</t>
+  </si>
+  <si>
+    <t>INC44624868</t>
   </si>
   <si>
     <t>Kostovski, Simon</t>
   </si>
   <si>
-    <t>please update the status for DP 31723 document to posted, it has been already approved</t>
-  </si>
-  <si>
-    <t>3014 - SIMEA BUZ</t>
+    <t>40042- WF not started for Unplanned delivery costs posted in amount of 350 eur.</t>
+  </si>
+  <si>
+    <t>WF not started after C block was assigned due to unplanned delivery costs. The WF should have started by design. (the document was now reposted for payment purposes but the cause should be investigated)</t>
+  </si>
+  <si>
+    <t>INC44639486</t>
+  </si>
+  <si>
+    <t>Pereira Dias Palmeiro Tavares, Maria Sofia</t>
+  </si>
+  <si>
+    <t>3011: New type of PO this FY - Limit Order process</t>
+  </si>
+  <si>
+    <t>XXFLAGXX - 0000 Placeholder for all not listed ARE – replaced automatically by your ARE</t>
+  </si>
+  <si>
+    <t>Dear team, I need your guidance regarding processing an invoice with this new type of PO (Limit Order process). We don't have a quantity specified in the PO, and when we process the invoice in VIM, the system requests a quantity. How can we process these invoices? Please see the attached example. Many thanks.</t>
+  </si>
+  <si>
+    <t>INC44615626</t>
+  </si>
+  <si>
+    <t>Cedidlo, Jiří</t>
+  </si>
+  <si>
+    <t>DP 47818</t>
   </si>
   <si>
     <t>4 - Low</t>
   </si>
   <si>
+    <t>Hello, please close the unclosed processes, change status to POSTED and transfer the document to ALL COMPLETED for document DP 47818.
+Many thanks.</t>
+  </si>
+  <si>
+    <t>INC44640708</t>
+  </si>
+  <si>
+    <t>Baiao, Milene</t>
+  </si>
+  <si>
+    <t>3009 - Unable to post invoice</t>
+  </si>
+  <si>
+    <t>In VIM we are not able to post invoice. 
+Error in the attached screenshtot.</t>
+  </si>
+  <si>
+    <t>INC44640838</t>
+  </si>
+  <si>
+    <t>Hermes, Pauline</t>
+  </si>
+  <si>
+    <t>Rechnungen von Lieferanten werden nicht bearbeitet.</t>
+  </si>
+  <si>
+    <t>Ein Lieferant hat sich bei uns gemeldet. Dieser schickt die Rechnungen an wstech.invoices.3366.de@siemens.com. Leider bekommt der Lieferant dann immer eine Fehlermeldung. 
+Sehr geehrte Damen und Herren,
+Sie haben an uns ein / mehrere Dokument (e) per E-Mail geschickt. Diese(s) Dokument(e) wurde(n) von uns abgewiesen, da diese leider aus folgendem Grund / folgende Gründe nicht verarbeitet werden konnte(n):
+- Die E-Mail war mit einer digitalen Signatur versehen. Bitte senden Sie die E-Mail ohne digitale Signatur erneut an uns.
+Wir möchten Sie darauf hinweisen, dass es sich um eine maschinelle Verarbeitung handelt und Informationen in der E-Mail nicht berücksichtigt werden. 
+Bei Fragen stehen wir Ihnen jederzeit unter Adresse scanning-ger.gss@siemens.com zur Verfügung.</t>
+  </si>
+  <si>
+    <t>INC44640887</t>
+  </si>
+  <si>
+    <t>Solomon, Denisa Aritina</t>
+  </si>
+  <si>
+    <t>Invoice approver wrongly identified in VIM for SIBIU</t>
+  </si>
+  <si>
     <t>In Process</t>
   </si>
   <si>
     <t>Please provide details about the nature of your issue.
+Dear all,
+Please contact me and provide a list of persons from Sibiu (3014, C503) with approver role in VIM. 
 Description of the Issue
 Error message if any
 Did it work before?
@@ -107,124 +221,132 @@
 How many people are impacted?</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>INC44581236</t>
-  </si>
-  <si>
-    <t>Øhrgaard, Maria Karmark</t>
-  </si>
-  <si>
-    <t>Supplier credit note goes to wrong PO</t>
-  </si>
-  <si>
-    <t>XXFLAGXX - RCDK - Region Denmark</t>
-  </si>
-  <si>
-    <t>Closed</t>
+    <t>INC44646142</t>
+  </si>
+  <si>
+    <t>DP 43534</t>
+  </si>
+  <si>
+    <t>Hello, please close the unclosed processes and workflows, change status to POSTED and transfer the document to ALL COMPLETED for document DP 43534. Full credit note for this invoice is posted, invoice is already cleared. Many thanks. Jiri Cedidlo</t>
+  </si>
+  <si>
+    <t>INC44646334</t>
+  </si>
+  <si>
+    <t>Moest, Tobias</t>
+  </si>
+  <si>
+    <t>S4P 100 VIM - Workflow Step Bezeichnung falsch</t>
+  </si>
+  <si>
+    <t>7998 - Siemens AG - SRE HQ</t>
+  </si>
+  <si>
+    <t>Offenbar wird in VIM im Freigabeworkflow der Workflow Step falsch angezeigt, was zu Verwirrung und Auswahl unpassender Freigeber führt. Beispiel ist VIM Vorgang 45503 - siehe Screenshots, bei dem  als Text "Technical Approval" stand. Laut VIM Analytics befindet sich der Vorgang aber im SChritt für die kaufmännische Freigabe, was dazu passt, dass beim WEiterleiten des Vorgangs auch nur Personen mit kaufmännischer Freigabeberechtigung (gemäß SAT) ausgewählt werden konnten.
+Ziel muss sein, dass immer die richtige Schrittbezeichnung angegeben wird!</t>
+  </si>
+  <si>
+    <t>INC44647135</t>
+  </si>
+  <si>
+    <t>DP 51843</t>
+  </si>
+  <si>
+    <t>Hello, please close the unclosed processes and workflows, change status to POSTED and transfer the document to ALL COMPLETED for document DP 51843. It is correction posting of internal invoice, approval not needed. Many thanks. Jiri Cedidlo</t>
+  </si>
+  <si>
+    <t>INC44647847</t>
+  </si>
+  <si>
+    <t>Piedade, Pedro</t>
+  </si>
+  <si>
+    <t>VIM doc didn't route to correct approver</t>
   </si>
   <si>
     <t>Please provide details about the nature of your issue.
-Description of the Issue
-Creditnote goes to other project than account assignment on PO
-Did it work before?
-yes
-Please see attached</t>
-  </si>
-  <si>
-    <t>INC44557114</t>
-  </si>
-  <si>
-    <t>Tsakova, Konstantina</t>
-  </si>
-  <si>
-    <t>Don't receive attachments in email</t>
-  </si>
-  <si>
-    <t>3 - Medium</t>
-  </si>
-  <si>
-    <t>Please provide details about the nature of your issue.
-There is a common mailbox, where we receives legal Romanian invoices applicable for 3014,  Sibiu, Romania 
-Description of the Issue - the issue is that all invoices in this email are sent by carrier via email and the PDF attachment is there. I will upload an example. The things is that only for Athos carrier, Sibiu, there is no attachment. The issue might be with MP1 cockpit, however the colleague responsible does not see an issue with it. This situation is for months and this is a roadblock that needs to be corrected, please. Here is the common mailbox: anaf.simea.ro@siemens.com. 
-Error message if any
-Did it work before? - never
-What was being done when the issue occurred? 
-What is the impact of the issue? (is the user able/unable to work?) - 
-When did the issue first occur? - since we received their first invoice in this mailbox - 25.11.2025
-Can the issue be replicated? How?
-How many people are impacted? -</t>
-  </si>
-  <si>
-    <t>Ignore</t>
-  </si>
-  <si>
-    <t>INC44475191</t>
-  </si>
-  <si>
-    <t>Piedade, Pedro</t>
-  </si>
-  <si>
-    <t>Tax code is inconsistent in VIM when compared with PO</t>
-  </si>
-  <si>
-    <t>3012 - Siemens Mobility A/S</t>
-  </si>
-  <si>
-    <t>Please provide details about the nature of your issue.
-We have found examples where the PO was created with tax code NQ, but then is switched to VD when invoice is uploaded to VIM. One such case is with doc 39989. We can see the original values are set as Tax Code VD, therefore there was no manual adjustment, it’s what the system is deriving. Why is that? This can generate lots of errors on the VAT Tax report if there’s an auto posting and these situations are no identified. Relevant screenshots in attachment.</t>
-  </si>
-  <si>
-    <t>INC44247133</t>
-  </si>
-  <si>
-    <t>Polanská, Pavlína</t>
-  </si>
-  <si>
-    <t>Inbox don't work properly</t>
-  </si>
-  <si>
-    <t>XXFLAGXX - 0000 Placeholder for all not listed ARE – replaced automatically by your ARE</t>
-  </si>
-  <si>
-    <t>If I go in to the inbox to see the invoices, it doesn't work properly, I cant see the whole invoice and if I click somewhere it goes back and so on. I can't do anything in the inbox.
-I'm still kind of new in Sherpa, i overtook the responsibilities from collegue from 1.10.2025 and since then it doesnt work properly.</t>
-  </si>
-  <si>
-    <t>INC44233598</t>
-  </si>
-  <si>
-    <t>Prasad K, Nagendra</t>
-  </si>
-  <si>
-    <t>Vendor bills on ISD registration not getting captured.</t>
-  </si>
-  <si>
-    <t>3368 – STSPL India</t>
-  </si>
-  <si>
-    <t>Hi Team,
-we have an ISD (Input Service Distributor) registration for common services such as insurance, audit fees, advertising etc. For such services, vendors are required to raise invoices against the ISD GST registration.
-Currently, due to system controls in VIM, we are unable to post invoices directly to the ISD registration. As a temporary workaround, the team will continue posting these invoices to the “KA” registration as an exception to ensure that critical payments—such as insurance—are processed within the cutoff timelines.
-To maintain compliance, a weekly report will be shared with the CFT team, which will serve as the basis for filing the necessary returns.
-Since this is only an interim solution, we request that the required changes be implemented in Sherpa X at the earliest, so that invoices can be booked directly against the ISD GSTIN.
-Please refer enclosed email for more details.
-Thank you</t>
-  </si>
-  <si>
-    <t>INC43708822</t>
-  </si>
-  <si>
-    <t>Wessner, Anna</t>
-  </si>
-  <si>
-    <t>No transparency in Order Confirmation Workflow</t>
-  </si>
-  <si>
-    <t>When an Order Confirmation Workflow is started we need to see which person currently is assigned to accept it and at which step, eg:
-1. Step: Not completed - Price deviation (GID of current user to accept)
-2. Step: Not completed - delivery date deviation (GID of User who the workflow will go to)</t>
+We have an invoice which was posted on 05.02.2025 and was waiting for GR to be posted, which hasn't occurred yet. However afted the 2 days normal wait for GR posting VIM did not route to the PO Requisitioner even though it's on the PO field. Why isn't this going automatically? Is there anything we can do to increase this automation?
+Also, when trying to manually route the invoice for approval the system doesn't show the options, they appear as blank. All screenshots are attached for referece.</t>
+  </si>
+  <si>
+    <t>INC44648228</t>
+  </si>
+  <si>
+    <t>Krňávková, Jitka</t>
+  </si>
+  <si>
+    <t>Stop AIF-Verarbeitung IDOCs an Ultimo 27.2.2026   18:00 Uhr</t>
+  </si>
+  <si>
+    <t>Lieber Uli, 
+bitte bei diesen BUK 
+3003
+3372
+3373
+3385
+3386
+3374
+3375
+3376
+3377
+3378
+3379
+3380
+3381
+3382
+7998
+460Q
+490C
+496Q
+die AiF am Freitag, den 27.2.2026, ab 18 Uhr stopen (Parameter für INVOIC IN (=Direction“ 2) und E (=Extern)  auf „Y“ setzen, d.h.)
+Bitte die Einträge wieder auf „ N“ ab 2. März setzen. (keine Stunde, kann sein wie möglich). 
+Danke schön
+Jitka</t>
+  </si>
+  <si>
+    <t>INC44649401</t>
+  </si>
+  <si>
+    <t>Mejia-Matos, Laura-Cristina</t>
+  </si>
+  <si>
+    <t>unable to approve document in workflow</t>
+  </si>
+  <si>
+    <t>unable to approve invoice in worflow, doc ID049118, please see screenshot</t>
+  </si>
+  <si>
+    <t>INC44653814</t>
+  </si>
+  <si>
+    <t>Cajtchamlová, Martina</t>
+  </si>
+  <si>
+    <t>add vendor 1000019213 to the table to allow posting with multiple POs</t>
+  </si>
+  <si>
+    <t>please add vendor 1000019213 to the table to allow posting with multiple POs</t>
+  </si>
+  <si>
+    <t>INC44653954</t>
+  </si>
+  <si>
+    <t>3014 - VIM DP 44471 stucked with SAP WFRT agent since 29/1/2026 - please restart approval workflow</t>
+  </si>
+  <si>
+    <t>Dear colleagues, please help with restarting workflow for DP 44471 that is stucedk in SAP WFRT workflow since 29/1/2026. This needs to be sent to price difference workflow.
+Thank you and kind regards
+Ivana</t>
+  </si>
+  <si>
+    <t>INC44654083</t>
+  </si>
+  <si>
+    <t>3014 - Credit note DP 32612 blocked with R with SAP WFRT agent</t>
+  </si>
+  <si>
+    <t>Dear colleagues,
+Please close down workflow for DP 32612 (credit note) that is stucked with SAP WFRT agent and unblock the document. Thank  you</t>
   </si>
 </sst>
 </file>
@@ -295,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -363,6 +485,116 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M2" t="n" s="2">
+        <v>45905.659583333334</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="T2" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="M3" t="n" s="2">
+        <v>46038.33106481482</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M4" t="n" s="2">
+        <v>46072.53946759259</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="M5" t="n" s="2">
+        <v>46076.53240740741</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -370,7 +602,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -440,28 +672,28 @@
     </row>
     <row r="2">
       <c r="B2" t="s" s="0">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="0">
         <v>23</v>
       </c>
       <c r="M2" t="n" s="4">
-        <v>46072.47770833333</v>
+        <v>46070.62741898148</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s" s="0">
         <v>25</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s" s="0">
         <v>27</v>
@@ -469,179 +701,338 @@
     </row>
     <row r="3">
       <c r="B3" t="s" s="0">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="M3" t="n" s="4">
-        <v>46062.32334490741</v>
+        <v>46076.62976851852</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="R3" t="s" s="0">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s" s="0">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="M4" t="n" s="4">
-        <v>46056.46460648148</v>
+        <v>46076.63997685185</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s" s="0">
         <v>25</v>
       </c>
       <c r="R4" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="T4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="U4" t="s" s="0">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s" s="0">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="M5" t="n" s="4">
-        <v>46036.59112268518</v>
+        <v>46076.64375</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="R5" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="U5" t="s" s="0">
-        <v>39</v>
+        <v>59</v>
+      </c>
+      <c r="T5" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M6" t="n" s="4">
+        <v>46077.344375</v>
+      </c>
+      <c r="N6" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="I6" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="M6" t="n" s="4">
-        <v>45992.610983796294</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>37</v>
-      </c>
       <c r="O6" t="s" s="0">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="R6" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="U6" t="s" s="0">
-        <v>39</v>
+        <v>62</v>
+      </c>
+      <c r="T6" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s" s="0">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="M7" t="n" s="4">
-        <v>45989.423368055555</v>
+        <v>46077.356099537035</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="U7" t="s" s="0">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="S7" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s" s="0">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s" s="0">
         <v>23</v>
       </c>
       <c r="M8" t="n" s="4">
-        <v>45919.32275462963</v>
+        <v>46077.41128472222</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O8" t="s" s="0">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="R8" t="s" s="0">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="T8" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="U8" t="s" s="0">
-        <v>39</v>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="M9" t="n" s="4">
+        <v>46077.45832175926</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="M10" t="n" s="4">
+        <v>46077.487662037034</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R10" t="s" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="L11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M11" t="n" s="4">
+        <v>46077.576574074075</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R11" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="T11" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M12" t="n" s="4">
+        <v>46078.323379629626</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="R12" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="T12" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="L13" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M13" t="n" s="4">
+        <v>46078.33315972222</v>
+      </c>
+      <c r="N13" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R13" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="T13" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="I14" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="L14" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="M14" t="n" s="4">
+        <v>46078.34185185185</v>
+      </c>
+      <c r="N14" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="R14" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="T14" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>